<commit_message>
update to hand picked
</commit_message>
<xml_diff>
--- a/output/plotassociations.xlsx
+++ b/output/plotassociations.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace2\USNVC\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{69BFE6EE-A3E9-4F6A-81D4-5A969C86AA65}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEB8FD1-3138-4F52-884E-C572BA2DC58A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plotassociations" sheetId="1" r:id="rId1"/>
@@ -259,7 +259,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1093,12 +1093,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41:C44"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1127,92 +1127,92 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>688421</v>
+        <v>686814</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>688421</v>
+        <v>686869</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>689615</v>
+      </c>
+      <c r="E4" t="s">
         <v>4</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>688421</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>688421</v>
+        <v>689615</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>688675</v>
+        <v>689615</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1221,123 +1221,123 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>686814</v>
+        <v>689615</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>686814</v>
+        <v>688421</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>686814</v>
+        <v>683201</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>686814</v>
+        <v>686101</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>686814</v>
+        <v>686190</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>686814</v>
+        <v>892928</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>686814</v>
+        <v>688421</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
         <v>2</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
       </c>
       <c r="D14">
         <v>683201</v>
@@ -1348,7 +1348,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -1365,7 +1365,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -1382,7 +1382,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -1391,628 +1391,628 @@
         <v>2</v>
       </c>
       <c r="D17">
-        <v>683201</v>
+        <v>686869</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
         <v>2</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
       <c r="D18">
-        <v>686101</v>
+        <v>686869</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D19">
-        <v>686101</v>
+        <v>686869</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D20">
-        <v>687693</v>
+        <v>686869</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>687693</v>
+        <v>686869</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D22">
-        <v>687693</v>
+        <v>688421</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>687693</v>
+        <v>686814</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B24">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24">
-        <v>687693</v>
+        <v>686814</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="B25">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D25">
-        <v>687693</v>
+        <v>686814</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C26">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D26">
-        <v>687693</v>
+        <v>686814</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D27">
-        <v>686869</v>
+        <v>686814</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
         <v>3</v>
       </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
       <c r="D28">
-        <v>686869</v>
+        <v>686814</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
         <v>3</v>
       </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
       <c r="D29">
-        <v>686869</v>
+        <v>685467</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
         <v>3</v>
       </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
       <c r="D30">
-        <v>686869</v>
+        <v>685467</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
         <v>3</v>
       </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
       <c r="D31">
-        <v>686869</v>
+        <v>683742</v>
       </c>
       <c r="E31" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D32">
-        <v>686869</v>
+        <v>687693</v>
       </c>
       <c r="E32" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D33">
-        <v>685728</v>
+        <v>687693</v>
       </c>
       <c r="E33" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D34">
-        <v>686190</v>
+        <v>687693</v>
       </c>
       <c r="E34" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D35">
-        <v>892928</v>
+        <v>687693</v>
       </c>
       <c r="E35" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B36">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C36">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D36">
-        <v>689089</v>
+        <v>685728</v>
       </c>
       <c r="E36" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="B37">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C37">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D37">
-        <v>689089</v>
+        <v>685380</v>
       </c>
       <c r="E37" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B38">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C38">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D38">
-        <v>689089</v>
+        <v>686421</v>
       </c>
       <c r="E38" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D39">
-        <v>793415</v>
+        <v>689103</v>
       </c>
       <c r="E39" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B40">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C40">
         <v>7</v>
       </c>
       <c r="D40">
-        <v>793415</v>
+        <v>689818</v>
       </c>
       <c r="E40" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D41">
-        <v>689615</v>
+        <v>689818</v>
       </c>
       <c r="E41" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D42">
-        <v>689615</v>
+        <v>686101</v>
       </c>
       <c r="E42" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43">
-        <v>689615</v>
+        <v>687693</v>
       </c>
       <c r="E43" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44">
-        <v>689615</v>
+        <v>687693</v>
       </c>
       <c r="E44" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C45">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D45">
-        <v>685380</v>
+        <v>687693</v>
       </c>
       <c r="E45" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="B46">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C46">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D46">
-        <v>686788</v>
+        <v>793415</v>
       </c>
       <c r="E46" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C47">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D47">
-        <v>685467</v>
+        <v>793415</v>
       </c>
       <c r="E47" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B48">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C48">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D48">
-        <v>685467</v>
+        <v>688421</v>
       </c>
       <c r="E48" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B49">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C49">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D49">
-        <v>683742</v>
+        <v>688675</v>
       </c>
       <c r="E49" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B50">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C50">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D50">
-        <v>686421</v>
+        <v>689089</v>
       </c>
       <c r="E50" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B51">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C51">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D51">
-        <v>689103</v>
+        <v>689089</v>
       </c>
       <c r="E51" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B52">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C52">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D52">
-        <v>689818</v>
+        <v>689089</v>
       </c>
       <c r="E52" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B53">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C53">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D53">
-        <v>689818</v>
+        <v>686788</v>
       </c>
       <c r="E53" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E53">
+  <autoFilter ref="A1:E53" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E53">
-      <sortCondition ref="E1:E53"/>
+      <sortCondition ref="B1:B53"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>